<commit_message>
changes done as change in dataset
</commit_message>
<xml_diff>
--- a/Atlique_FMCG_promotional_analysis/recommended insights/promotion_performance/campaign_sales_by_city.xlsx
+++ b/Atlique_FMCG_promotional_analysis/recommended insights/promotion_performance/campaign_sales_by_city.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Vivek\sql\SQL\Atlique_FMCG_promotional_analysis\recommended insights\promotion_performance\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BB6678D-3C2B-47FB-997B-ADE4F035AABE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D04ACE4-CAF9-4EA3-8167-34E1B6D84E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="16">
   <si>
     <t>city</t>
   </si>
@@ -693,49 +693,7 @@
           </a:effectLst>
         </c:spPr>
         <c:marker>
-          <c:symbol val="circle"/>
-          <c:size val="6"/>
-          <c:spPr>
-            <a:gradFill rotWithShape="1">
-              <a:gsLst>
-                <a:gs pos="0">
-                  <a:schemeClr val="accent4">
-                    <a:satMod val="103000"/>
-                    <a:lumMod val="102000"/>
-                    <a:tint val="94000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="50000">
-                  <a:schemeClr val="accent4">
-                    <a:satMod val="110000"/>
-                    <a:lumMod val="100000"/>
-                    <a:shade val="100000"/>
-                  </a:schemeClr>
-                </a:gs>
-                <a:gs pos="100000">
-                  <a:schemeClr val="accent4">
-                    <a:lumMod val="99000"/>
-                    <a:satMod val="120000"/>
-                    <a:shade val="78000"/>
-                  </a:schemeClr>
-                </a:gs>
-              </a:gsLst>
-              <a:lin ang="5400000" scaled="0"/>
-            </a:gradFill>
-            <a:ln w="9525">
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst>
-              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
-                <a:srgbClr val="000000">
-                  <a:alpha val="63000"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
-          </c:spPr>
+          <c:symbol val="none"/>
         </c:marker>
         <c:dLbl>
           <c:idx val="0"/>
@@ -895,9 +853,9 @@
           </c:dLbls>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>Sheet1!$A$4:$B$5</c:f>
+              <c:f>Sheet1!$A$4:$B$23</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="2"/>
+                <c:ptCount val="20"/>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Diwali</c:v>
@@ -905,10 +863,91 @@
                   <c:pt idx="1">
                     <c:v>Sankranti</c:v>
                   </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Diwali</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Sankranti</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Diwali</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Sankranti</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Diwali</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Sankranti</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Diwali</c:v>
+                  </c:pt>
+                  <c:pt idx="9">
+                    <c:v>Sankranti</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Diwali</c:v>
+                  </c:pt>
+                  <c:pt idx="11">
+                    <c:v>Sankranti</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Diwali</c:v>
+                  </c:pt>
+                  <c:pt idx="13">
+                    <c:v>Sankranti</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>Diwali</c:v>
+                  </c:pt>
+                  <c:pt idx="15">
+                    <c:v>Sankranti</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>Diwali</c:v>
+                  </c:pt>
+                  <c:pt idx="17">
+                    <c:v>Sankranti</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>Diwali</c:v>
+                  </c:pt>
+                  <c:pt idx="19">
+                    <c:v>Sankranti</c:v>
+                  </c:pt>
                 </c:lvl>
                 <c:lvl>
                   <c:pt idx="0">
                     <c:v>Bengaluru</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>Chennai</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Coimbatore</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Hyderabad</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>Madurai</c:v>
+                  </c:pt>
+                  <c:pt idx="10">
+                    <c:v>Mangalore</c:v>
+                  </c:pt>
+                  <c:pt idx="12">
+                    <c:v>Mysuru</c:v>
+                  </c:pt>
+                  <c:pt idx="14">
+                    <c:v>Trivandrum</c:v>
+                  </c:pt>
+                  <c:pt idx="16">
+                    <c:v>Vijayawada</c:v>
+                  </c:pt>
+                  <c:pt idx="18">
+                    <c:v>Visakhapatnam</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -916,15 +955,69 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$C$4:$C$5</c:f>
+              <c:f>Sheet1!$C$4:$C$23</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="20"/>
                 <c:pt idx="0">
                   <c:v>41.85</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>30.56</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>33.119999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24.82</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>14.7</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.64</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>26.57</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>19.690000000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>13.64</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.42</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.04</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.1399999999999997</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>16.48</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10.84</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>3.79</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>3.03</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.57</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>13.04</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>9.67</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -954,6 +1047,72 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IN"/>
+                  <a:t>city</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-IN" baseline="0"/>
+                  <a:t> and corresponding festival</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-IN"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.40313059440272903"/>
+              <c:y val="0.81844516229525199"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1004,6 +1163,64 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-IN"/>
+                  <a:t>Revenue</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-IN" baseline="0"/>
+                  <a:t> in millions</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-IN"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1048,6 +1265,16 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.70452684493831674"/>
+          <c:y val="9.386062384212622E-2"/>
+          <c:w val="4.0544789171647923E-2"/>
+          <c:h val="5.2987947460643538E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1828,20 +2055,20 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable9" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="8" indent="0" compact="0" compactData="0" multipleFieldFilters="0" chartFormat="4">
-  <location ref="A3:C5" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
+  <location ref="A3:C23" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" compact="0" outline="0" showAll="0" defaultSubtotal="0">
       <items count="10">
         <item x="0"/>
-        <item h="1" x="1"/>
-        <item h="1" x="2"/>
-        <item h="1" x="3"/>
-        <item h="1" x="4"/>
-        <item h="1" x="5"/>
-        <item h="1" x="6"/>
-        <item h="1" x="7"/>
-        <item h="1" x="8"/>
-        <item h="1" x="9"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
       </items>
       <extLst>
         <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{2946ED86-A175-432a-8AC1-64E0C546D7DE}">
@@ -1872,9 +2099,72 @@
     <field x="0"/>
     <field x="1"/>
   </rowFields>
-  <rowItems count="2">
+  <rowItems count="20">
     <i>
       <x/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="1"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="3"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="4"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="5"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="6"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="7"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="8"/>
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="9"/>
       <x/>
     </i>
     <i r="1">
@@ -1887,27 +2177,12 @@
   <dataFields count="1">
     <dataField name="Sum of total_revenue_generated_in_mil" fld="2" baseField="0" baseItem="0"/>
   </dataFields>
-  <chartFormats count="2">
+  <chartFormats count="1">
     <chartFormat chart="0" format="1" series="1">
       <pivotArea type="data" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="1" selected="0">
             <x v="0"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </chartFormat>
-    <chartFormat chart="0" format="2">
-      <pivotArea type="data" outline="0" fieldPosition="0">
-        <references count="3">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="0" count="1" selected="0">
-            <x v="0"/>
-          </reference>
-          <reference field="1" count="1" selected="0">
-            <x v="1"/>
           </reference>
         </references>
       </pivotArea>
@@ -2222,7 +2497,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A3:C5"/>
+  <dimension ref="A3:C23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K16" sqref="K16"/>
@@ -2266,6 +2541,204 @@
       </c>
       <c r="C5" s="2">
         <v>30.56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2">
+        <v>33.119999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2">
+        <v>24.82</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2">
+        <v>14.7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="2">
+        <v>11.64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="2">
+        <v>26.57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="2">
+        <v>19.690000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4</v>
+      </c>
+      <c r="C12" s="2">
+        <v>13.64</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+      <c r="C13" s="2">
+        <v>9.42</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="2">
+        <v>6.04</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>5</v>
+      </c>
+      <c r="C15" s="2">
+        <v>4.1399999999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16" s="2">
+        <v>16.48</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>11</v>
+      </c>
+      <c r="B17" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="2">
+        <v>10.84</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B18" t="s">
+        <v>4</v>
+      </c>
+      <c r="C18" s="2">
+        <v>3.79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="2">
+        <v>3.03</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C20" s="2">
+        <v>4.57</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21" s="2">
+        <v>3.2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" t="s">
+        <v>4</v>
+      </c>
+      <c r="C22" s="2">
+        <v>13.04</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="2">
+        <v>9.67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>